<commit_message>
can load special packages into a special list on trucks to ensure they are there, to then be loaded onto truck's regular list
</commit_message>
<xml_diff>
--- a/data/all_delivery_data_backup.xlsx
+++ b/data/all_delivery_data_backup.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adamm\PycharmProjects\TravelingDeliveryman\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{0DD9CD97-9C2A-4265-9FBD-FA0633805659}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{5E3E04D2-40EB-421E-BB16-A11584D2EEC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="4200" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="34620" windowHeight="14020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="package_data" sheetId="4" r:id="rId1"/>
@@ -20,6 +20,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2">address_data!$A$1:$C$28</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">package_data!$A$1:$H$41</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="74">
   <si>
     <t>address_id</t>
   </si>
@@ -264,9 +265,6 @@
   </si>
   <si>
     <t>location_name</t>
-  </si>
-  <si>
-    <t>address_available_time</t>
   </si>
 </sst>
 </file>
@@ -532,7 +530,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -601,10 +599,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -885,10 +879,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{259C2A56-3C60-479F-941A-D591511CBD81}">
-  <dimension ref="A1:I41"/>
+  <dimension ref="A1:H41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="W12" sqref="W12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -899,7 +893,7 @@
     <col min="7" max="7" width="13.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="36.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" ht="24.5" x14ac:dyDescent="0.35">
       <c r="A1" s="17" t="s">
         <v>1</v>
       </c>
@@ -924,11 +918,8 @@
       <c r="H1" s="22" t="s">
         <v>71</v>
       </c>
-      <c r="I1" s="26" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="18">
         <v>1</v>
       </c>
@@ -953,11 +944,8 @@
       <c r="H2" t="b">
         <v>0</v>
       </c>
-      <c r="I2" s="27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="18">
         <v>2</v>
       </c>
@@ -982,11 +970,8 @@
       <c r="H3" t="b">
         <v>0</v>
       </c>
-      <c r="I3" s="27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="18">
         <v>3</v>
       </c>
@@ -1011,11 +996,8 @@
       <c r="H4" t="b">
         <v>0</v>
       </c>
-      <c r="I4" s="27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" s="18">
         <v>4</v>
       </c>
@@ -1040,11 +1022,8 @@
       <c r="H5" t="b">
         <v>0</v>
       </c>
-      <c r="I5" s="27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" s="18">
         <v>5</v>
       </c>
@@ -1069,11 +1048,8 @@
       <c r="H6" t="b">
         <v>0</v>
       </c>
-      <c r="I6" s="27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" s="18">
         <v>6</v>
       </c>
@@ -1098,11 +1074,8 @@
       <c r="H7" t="b">
         <v>0</v>
       </c>
-      <c r="I7" s="27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" s="18">
         <v>7</v>
       </c>
@@ -1127,11 +1100,8 @@
       <c r="H8" t="b">
         <v>0</v>
       </c>
-      <c r="I8" s="27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" s="18">
         <v>8</v>
       </c>
@@ -1156,11 +1126,8 @@
       <c r="H9" t="b">
         <v>0</v>
       </c>
-      <c r="I9" s="27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" s="18">
         <v>9</v>
       </c>
@@ -1185,11 +1152,8 @@
       <c r="H10" t="b">
         <v>1</v>
       </c>
-      <c r="I10" s="27">
-        <v>0.43055555555555558</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" s="18">
         <v>10</v>
       </c>
@@ -1214,11 +1178,8 @@
       <c r="H11" t="b">
         <v>0</v>
       </c>
-      <c r="I11" s="27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" s="18">
         <v>11</v>
       </c>
@@ -1243,11 +1204,8 @@
       <c r="H12" t="b">
         <v>0</v>
       </c>
-      <c r="I12" s="27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" s="18">
         <v>12</v>
       </c>
@@ -1272,11 +1230,8 @@
       <c r="H13" t="b">
         <v>0</v>
       </c>
-      <c r="I13" s="27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" s="18">
         <v>13</v>
       </c>
@@ -1301,11 +1256,8 @@
       <c r="H14" t="b">
         <v>0</v>
       </c>
-      <c r="I14" s="27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" s="18">
         <v>14</v>
       </c>
@@ -1330,11 +1282,8 @@
       <c r="H15" t="b">
         <v>0</v>
       </c>
-      <c r="I15" s="27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" s="18">
         <v>15</v>
       </c>
@@ -1359,11 +1308,8 @@
       <c r="H16" t="b">
         <v>0</v>
       </c>
-      <c r="I16" s="27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17" s="18">
         <v>16</v>
       </c>
@@ -1388,11 +1334,8 @@
       <c r="H17" t="b">
         <v>0</v>
       </c>
-      <c r="I17" s="27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A18" s="18">
         <v>17</v>
       </c>
@@ -1417,11 +1360,8 @@
       <c r="H18" t="b">
         <v>0</v>
       </c>
-      <c r="I18" s="27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A19" s="18">
         <v>18</v>
       </c>
@@ -1446,11 +1386,8 @@
       <c r="H19" t="b">
         <v>0</v>
       </c>
-      <c r="I19" s="27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A20" s="18">
         <v>19</v>
       </c>
@@ -1475,11 +1412,8 @@
       <c r="H20" t="b">
         <v>0</v>
       </c>
-      <c r="I20" s="27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A21" s="18">
         <v>20</v>
       </c>
@@ -1504,11 +1438,8 @@
       <c r="H21" t="b">
         <v>0</v>
       </c>
-      <c r="I21" s="27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A22" s="18">
         <v>21</v>
       </c>
@@ -1533,11 +1464,8 @@
       <c r="H22" t="b">
         <v>0</v>
       </c>
-      <c r="I22" s="27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A23" s="18">
         <v>22</v>
       </c>
@@ -1562,11 +1490,8 @@
       <c r="H23" t="b">
         <v>0</v>
       </c>
-      <c r="I23" s="27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A24" s="18">
         <v>23</v>
       </c>
@@ -1591,11 +1516,8 @@
       <c r="H24" t="b">
         <v>0</v>
       </c>
-      <c r="I24" s="27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A25" s="18">
         <v>24</v>
       </c>
@@ -1620,11 +1542,8 @@
       <c r="H25" t="b">
         <v>0</v>
       </c>
-      <c r="I25" s="27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A26" s="18">
         <v>25</v>
       </c>
@@ -1649,11 +1568,8 @@
       <c r="H26" t="b">
         <v>0</v>
       </c>
-      <c r="I26" s="27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A27" s="18">
         <v>26</v>
       </c>
@@ -1678,11 +1594,8 @@
       <c r="H27" t="b">
         <v>0</v>
       </c>
-      <c r="I27" s="27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A28" s="18">
         <v>27</v>
       </c>
@@ -1707,11 +1620,8 @@
       <c r="H28" t="b">
         <v>0</v>
       </c>
-      <c r="I28" s="27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A29" s="18">
         <v>28</v>
       </c>
@@ -1736,11 +1646,8 @@
       <c r="H29" t="b">
         <v>0</v>
       </c>
-      <c r="I29" s="27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A30" s="18">
         <v>29</v>
       </c>
@@ -1765,11 +1672,8 @@
       <c r="H30" t="b">
         <v>0</v>
       </c>
-      <c r="I30" s="27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A31" s="18">
         <v>30</v>
       </c>
@@ -1794,11 +1698,8 @@
       <c r="H31" t="b">
         <v>0</v>
       </c>
-      <c r="I31" s="27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A32" s="18">
         <v>31</v>
       </c>
@@ -1823,11 +1724,8 @@
       <c r="H32" t="b">
         <v>0</v>
       </c>
-      <c r="I32" s="27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A33" s="18">
         <v>32</v>
       </c>
@@ -1852,11 +1750,8 @@
       <c r="H33" t="b">
         <v>0</v>
       </c>
-      <c r="I33" s="27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A34" s="18">
         <v>33</v>
       </c>
@@ -1881,11 +1776,8 @@
       <c r="H34" t="b">
         <v>0</v>
       </c>
-      <c r="I34" s="27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A35" s="18">
         <v>34</v>
       </c>
@@ -1910,11 +1802,8 @@
       <c r="H35" t="b">
         <v>0</v>
       </c>
-      <c r="I35" s="27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A36" s="18">
         <v>35</v>
       </c>
@@ -1939,11 +1828,8 @@
       <c r="H36" t="b">
         <v>0</v>
       </c>
-      <c r="I36" s="27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A37" s="18">
         <v>36</v>
       </c>
@@ -1968,11 +1854,8 @@
       <c r="H37" t="b">
         <v>0</v>
       </c>
-      <c r="I37" s="27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A38" s="18">
         <v>37</v>
       </c>
@@ -1997,11 +1880,8 @@
       <c r="H38" t="b">
         <v>0</v>
       </c>
-      <c r="I38" s="27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A39" s="18">
         <v>38</v>
       </c>
@@ -2026,11 +1906,8 @@
       <c r="H39" t="b">
         <v>0</v>
       </c>
-      <c r="I39" s="27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A40" s="18">
         <v>39</v>
       </c>
@@ -2055,11 +1932,8 @@
       <c r="H40" t="b">
         <v>0</v>
       </c>
-      <c r="I40" s="27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A41" s="18">
         <v>40</v>
       </c>
@@ -2084,11 +1958,9 @@
       <c r="H41" t="b">
         <v>0</v>
       </c>
-      <c r="I41" s="27">
-        <v>0</v>
-      </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:H41" xr:uid="{259C2A56-3C60-479F-941A-D591511CBD81}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
@@ -3825,8 +3697,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4222C95-8038-46BE-A878-DD9F1771B676}">
   <dimension ref="A1:F28"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>